<commit_message>
Home page loaded test case updated
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\zygalAutomation\zygal_connect_application\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22455" windowHeight="7560"/>
   </bookViews>
@@ -10,7 +15,6 @@
     <sheet name="loginData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +35,7 @@
     <t>OTP</t>
   </si>
   <si>
-    <t>ABC12</t>
+    <t>ABC123</t>
   </si>
 </sst>
 </file>
@@ -397,7 +401,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated report section and error handling
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -29,13 +29,13 @@
     <t>UserName</t>
   </si>
   <si>
-    <t>k.rush7999@gmail.com</t>
-  </si>
-  <si>
     <t>OTP</t>
   </si>
   <si>
     <t>ABC123</t>
+  </si>
+  <si>
+    <t>k.rush7999@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -401,7 +401,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,15 +415,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added method explanation for login flow
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -32,10 +32,10 @@
     <t>OTP</t>
   </si>
   <si>
-    <t>ABC123</t>
+    <t>k.rush7999@gmail.com</t>
   </si>
   <si>
-    <t>k.rush7999@gmail.com</t>
+    <t>X1Y2Z3</t>
   </si>
 </sst>
 </file>
@@ -401,7 +401,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,10 +420,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added invalid otp, invalid email and other test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>UserName</t>
   </si>
@@ -36,6 +36,12 @@
   </si>
   <si>
     <t>X1Y2Z3</t>
+  </si>
+  <si>
+    <t>k@gmail.com</t>
+  </si>
+  <si>
+    <t>XYZ123</t>
   </si>
 </sst>
 </file>
@@ -398,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,9 +432,18 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated in the report and added one step for not registred email
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>UserName</t>
   </si>
@@ -38,10 +38,13 @@
     <t>X1Y2Z3</t>
   </si>
   <si>
-    <t>k@gmail.com</t>
-  </si>
-  <si>
     <t>XYZ123</t>
+  </si>
+  <si>
+    <t>prashant</t>
+  </si>
+  <si>
+    <t>prashant@test.com</t>
   </si>
 </sst>
 </file>
@@ -404,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -434,16 +437,22 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId2" display="k@gmail.com"/>
+    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Resend OTP button test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>UserName</t>
   </si>
@@ -58,13 +58,46 @@
   </si>
   <si>
     <t>Expected Message</t>
+  </si>
+  <si>
+    <t>Email field cannot be empty</t>
+  </si>
+  <si>
+    <t>Invalid email address. Please enter a valid email</t>
+  </si>
+  <si>
+    <t>No such user found</t>
+  </si>
+  <si>
+    <t>Please enter valid OTP</t>
+  </si>
+  <si>
+    <t>Incorrect OTP</t>
+  </si>
+  <si>
+    <t>You have reached the maximum login attempts for the day. Please try again after 24 hours.</t>
+  </si>
+  <si>
+    <t>Kindly press the back button once more to exit the application</t>
+  </si>
+  <si>
+    <t>Access denied by firewall. Contact administrator.</t>
+  </si>
+  <si>
+    <t>Something went wrong</t>
+  </si>
+  <si>
+    <t>Session expired. Please login again</t>
+  </si>
+  <si>
+    <t>OTP sent successfully</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +112,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,9 +142,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -490,20 +536,80 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated resend otp button account block issue
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>UserName</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>OTP sent successfully</t>
+  </si>
+  <si>
+    <t>resend@g.io</t>
+  </si>
+  <si>
+    <t>Resend OTP test</t>
+  </si>
+  <si>
+    <t>Incorrrect otp tst</t>
+  </si>
+  <si>
+    <t>Max OTP retry limit reached. Please try again later</t>
   </si>
 </sst>
 </file>
@@ -466,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,6 +525,9 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -520,6 +535,14 @@
       </c>
       <c r="E6" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -529,6 +552,7 @@
     <hyperlink ref="A4" r:id="rId3"/>
     <hyperlink ref="A5" r:id="rId4"/>
     <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -536,7 +560,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
@@ -612,6 +636,11 @@
         <v>21</v>
       </c>
     </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
home page method updated
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -3,19 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\zygalAutomation\zygal_connect_application\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22455" windowHeight="7560" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21525" windowHeight="3600"/>
   </bookViews>
   <sheets>
     <sheet name="loginData" sheetId="1" r:id="rId1"/>
-    <sheet name="Message" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Message" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:P10"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>UserName</t>
   </si>
@@ -36,73 +33,82 @@
     <t>k.rush7999@gmail.com</t>
   </si>
   <si>
+    <t>XYZ123</t>
+  </si>
+  <si>
+    <t>prashant</t>
+  </si>
+  <si>
+    <t>prashant@test.com</t>
+  </si>
+  <si>
+    <t>p@gmail.com</t>
+  </si>
+  <si>
+    <t>udaleprashant@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin viewer account </t>
+  </si>
+  <si>
+    <t>Expected Message</t>
+  </si>
+  <si>
+    <t>Email field cannot be empty</t>
+  </si>
+  <si>
+    <t>Invalid email address. Please enter a valid email</t>
+  </si>
+  <si>
+    <t>No such user found</t>
+  </si>
+  <si>
+    <t>Please enter valid OTP</t>
+  </si>
+  <si>
+    <t>Incorrect OTP</t>
+  </si>
+  <si>
+    <t>You have reached the maximum login attempts for the day. Please try again after 24 hours.</t>
+  </si>
+  <si>
+    <t>Kindly press the back button once more to exit the application</t>
+  </si>
+  <si>
+    <t>Access denied by firewall. Contact administrator.</t>
+  </si>
+  <si>
+    <t>Something went wrong</t>
+  </si>
+  <si>
+    <t>Session expired. Please login again</t>
+  </si>
+  <si>
+    <t>OTP sent successfully</t>
+  </si>
+  <si>
+    <t>resend@g.io</t>
+  </si>
+  <si>
+    <t>Resend OTP test</t>
+  </si>
+  <si>
+    <t>Incorrrect otp tst</t>
+  </si>
+  <si>
+    <t>Max OTP retry limit reached. Please try again later</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not registred account check </t>
+  </si>
+  <si>
+    <t>Account block check for incorrect OTP so DND</t>
+  </si>
+  <si>
+    <t>Automation Test</t>
+  </si>
+  <si>
     <t>X1Y2Z3</t>
-  </si>
-  <si>
-    <t>XYZ123</t>
-  </si>
-  <si>
-    <t>prashant</t>
-  </si>
-  <si>
-    <t>prashant@test.com</t>
-  </si>
-  <si>
-    <t>p@gmail.com</t>
-  </si>
-  <si>
-    <t>udaleprashant@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admin viewer account </t>
-  </si>
-  <si>
-    <t>Expected Message</t>
-  </si>
-  <si>
-    <t>Email field cannot be empty</t>
-  </si>
-  <si>
-    <t>Invalid email address. Please enter a valid email</t>
-  </si>
-  <si>
-    <t>No such user found</t>
-  </si>
-  <si>
-    <t>Please enter valid OTP</t>
-  </si>
-  <si>
-    <t>Incorrect OTP</t>
-  </si>
-  <si>
-    <t>You have reached the maximum login attempts for the day. Please try again after 24 hours.</t>
-  </si>
-  <si>
-    <t>Kindly press the back button once more to exit the application</t>
-  </si>
-  <si>
-    <t>Access denied by firewall. Contact administrator.</t>
-  </si>
-  <si>
-    <t>Something went wrong</t>
-  </si>
-  <si>
-    <t>Session expired. Please login again</t>
-  </si>
-  <si>
-    <t>OTP sent successfully</t>
-  </si>
-  <si>
-    <t>resend@g.io</t>
-  </si>
-  <si>
-    <t>Resend OTP test</t>
-  </si>
-  <si>
-    <t>Incorrrect otp tst</t>
-  </si>
-  <si>
-    <t>Max OTP retry limit reached. Please try again later</t>
   </si>
 </sst>
 </file>
@@ -154,7 +160,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -162,6 +168,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -480,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,44 +517,47 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
         <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
         <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -560,9 +575,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -573,72 +623,72 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated config flag and ran/executed all the test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21525" windowHeight="3600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21525" windowHeight="5775"/>
   </bookViews>
   <sheets>
     <sheet name="loginData" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>UserName</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Resend OTP test</t>
   </si>
   <si>
-    <t>Incorrrect otp tst</t>
-  </si>
-  <si>
     <t>Max OTP retry limit reached. Please try again later</t>
   </si>
   <si>
@@ -109,6 +106,12 @@
   </si>
   <si>
     <t>X1Y2Z3</t>
+  </si>
+  <si>
+    <t>Incorrrect otp test</t>
+  </si>
+  <si>
+    <t>p@g.com</t>
   </si>
 </sst>
 </file>
@@ -493,7 +496,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +520,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -533,15 +536,15 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -591,13 +594,13 @@
         <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -688,7 +691,7 @@
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>